<commit_message>
Add function to populate local impairment details report
</commit_message>
<xml_diff>
--- a/app/templates/reports/local_impairment_details_report.xlsx
+++ b/app/templates/reports/local_impairment_details_report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Dalex Finance</t>
   </si>
@@ -68,27 +68,6 @@
   </si>
   <si>
     <t xml:space="preserve">Provision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recovery rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20%</t>
   </si>
 </sst>
 </file>
@@ -99,11 +78,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -119,12 +99,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -176,33 +150,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -328,10 +298,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -351,169 +321,78 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="4"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
@@ -546,76 +425,11 @@
       <c r="J14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="4" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E18" s="4" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E19" s="4" t="n">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>